<commit_message>
Update edited session - 2025-09-06T10:32:25.733Z - Cache Bust ID: 1757154745733opnslqj6t
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2425_Pediatrics_scanner1757106499774_b238c595b84321b35b8e57610c49523d4e3b9b5b5d090923e9e54f4b929bedba.xlsx
+++ b/log_history/Y5_B2425_Pediatrics_scanner1757106499774_b238c595b84321b35b8e57610c49523d4e3b9b5b5d090923e9e54f4b929bedba.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,29 +422,9 @@
         <v>User</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>124578</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Pediatrics</v>
-      </c>
-      <c r="C2" t="str">
-        <v>06/09/2025</v>
-      </c>
-      <c r="D2" t="str">
-        <v>13:31:23</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F2" t="str">
-        <v>user@user.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>